<commit_message>
change vehicle to car, NOT run with truck
</commit_message>
<xml_diff>
--- a/Scripts/data/input_location_data.xlsx
+++ b/Scripts/data/input_location_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Funix\My project\Nam Project\python\CalcDistanceMatrixFromXY\Scripts\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SANG\Nam Project\python\CalcDistanceMatrixFromXY\Scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD971F7C-BD01-472B-8B97-322DB84D9511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D326E8-4390-4406-B31C-DC7A99FC51F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,8 +51,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -68,6 +74,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -99,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -111,6 +123,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,19 +430,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -438,236 +453,766 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="4">
-        <v>106.763047</v>
-      </c>
-      <c r="C2" s="4">
-        <v>10.631424000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="5">
+        <v>107.02427884232701</v>
+      </c>
+      <c r="C2" s="5">
+        <v>10.6072384967056</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>106.725171</v>
+        <v>107.2925092</v>
       </c>
       <c r="C3" s="4">
-        <v>10.666356</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.8382992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>106.729698</v>
+        <v>107.35621980000001</v>
       </c>
       <c r="C4" s="4">
-        <v>10.652474</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.792846600000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>106.724994</v>
+        <v>107.3237412</v>
       </c>
       <c r="C5" s="4">
-        <v>10.666641</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.723538400000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>106.703453</v>
+        <v>107.34938649999999</v>
       </c>
       <c r="C6" s="4">
-        <v>10.705958000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.741887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>106.71558400000001</v>
+        <v>107.35160310000001</v>
       </c>
       <c r="C7" s="4">
-        <v>10.657063000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.7319087</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>106.701396</v>
+        <v>107.35157599999999</v>
       </c>
       <c r="C8" s="4">
-        <v>10.679833</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.751467399999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>106.742086</v>
+        <v>107.35130100000001</v>
       </c>
       <c r="C9" s="4">
-        <v>10.687904</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.747577700000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>106.70314399999999</v>
+        <v>107.3512925</v>
       </c>
       <c r="C10" s="4">
-        <v>10.706704999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.731367199999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>106.628766</v>
+        <v>107.3435336</v>
       </c>
       <c r="C11" s="4">
-        <v>10.882154</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.7628431</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>106.775176</v>
+        <v>107.3505794</v>
       </c>
       <c r="C12" s="4">
-        <v>10.814462000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.767490499999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>106.69537800000001</v>
+        <v>107.3052122</v>
       </c>
       <c r="C13" s="4">
-        <v>10.666155</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.7559752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>106.74074299999999</v>
+        <v>107.37694449999999</v>
       </c>
       <c r="C14" s="4">
-        <v>10.693479999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.616922600000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>106.70234600000001</v>
+        <v>107.54477369999999</v>
       </c>
       <c r="C15" s="4">
-        <v>10.709409000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.559908500000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>106.698758</v>
+        <v>107.4345624</v>
       </c>
       <c r="C16" s="4">
-        <v>10.712911</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.548318399999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>106.73973599999999</v>
+        <v>107.3820486</v>
       </c>
       <c r="C17" s="4">
-        <v>10.69556</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.8409555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>106.719487</v>
+        <v>107.2201762</v>
       </c>
       <c r="C18" s="4">
-        <v>10.636101999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.791483700000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>106.726844</v>
+        <v>107.1871233</v>
       </c>
       <c r="C19" s="4">
-        <v>10.63245</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.8131679</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>106.7376459</v>
+        <v>107.28000299999999</v>
       </c>
       <c r="C20" s="4">
-        <v>10.7141956</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.872092</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>106.7159358</v>
+        <v>107.1602683</v>
       </c>
       <c r="C21" s="4">
-        <v>10.745618199999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10.8612799</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>106.7084131</v>
+        <v>107.2366997</v>
       </c>
       <c r="C22" s="4">
-        <v>10.8029288</v>
-      </c>
+        <v>10.8358981</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>107.2304671</v>
+      </c>
+      <c r="C23" s="4">
+        <v>10.8196677</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>107.229674</v>
+      </c>
+      <c r="C24" s="4">
+        <v>10.817656700000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="4">
+        <v>107.23253219999999</v>
+      </c>
+      <c r="C25" s="4">
+        <v>10.824465399999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
+        <v>107.2794317</v>
+      </c>
+      <c r="C26" s="4">
+        <v>10.696851799999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="4">
+        <v>107.2416711</v>
+      </c>
+      <c r="C27" s="4">
+        <v>10.722218099999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>107.2353122</v>
+      </c>
+      <c r="C28" s="4">
+        <v>10.7555388</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="4">
+        <v>107.2386992</v>
+      </c>
+      <c r="C29" s="4">
+        <v>10.702419300000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <v>107.24190919999999</v>
+      </c>
+      <c r="C30" s="4">
+        <v>10.631271699999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="4">
+        <v>107.07962790000001</v>
+      </c>
+      <c r="C31" s="4">
+        <v>10.6311929</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
+        <v>107.06150909999999</v>
+      </c>
+      <c r="C32" s="4">
+        <v>10.6270311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4">
+        <v>107.2035956</v>
+      </c>
+      <c r="C33" s="4">
+        <v>10.7406097</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
+        <v>107.1602683</v>
+      </c>
+      <c r="C34" s="4">
+        <v>10.730828199999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4">
+        <v>107.15105800000001</v>
+      </c>
+      <c r="C35" s="4">
+        <v>10.723762499999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="4">
+        <v>107.1535451</v>
+      </c>
+      <c r="C36" s="4">
+        <v>10.719318400000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="4">
+        <v>107.13278560000001</v>
+      </c>
+      <c r="C37" s="4">
+        <v>10.8292514</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
+        <v>107.0845808</v>
+      </c>
+      <c r="C38" s="4">
+        <v>10.817228800000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="4">
+        <v>107.03782630000001</v>
+      </c>
+      <c r="C39" s="4">
+        <v>10.998201699999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="4">
+        <v>107.31226359999999</v>
+      </c>
+      <c r="C40" s="4">
+        <v>10.807557900000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="4">
+        <v>107.29619529999999</v>
+      </c>
+      <c r="C41" s="4">
+        <v>10.815440600000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="4">
+        <v>107.29703499999999</v>
+      </c>
+      <c r="C42" s="4">
+        <v>10.834960000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="4">
+        <v>107.2838081</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10.902956400000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="4">
+        <v>107.3682</v>
+      </c>
+      <c r="C44" s="4">
+        <v>10.762578</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="4">
+        <v>107.332729</v>
+      </c>
+      <c r="C45" s="4">
+        <v>10.7147962</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="4">
+        <v>107.3257545</v>
+      </c>
+      <c r="C46" s="4">
+        <v>10.6997304</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="4">
+        <v>107.312364</v>
+      </c>
+      <c r="C47" s="4">
+        <v>10.67906</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="4">
+        <v>107.34070149999999</v>
+      </c>
+      <c r="C48" s="4">
+        <v>10.7179792</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="4">
+        <v>107.33578300000001</v>
+      </c>
+      <c r="C49" s="4">
+        <v>10.7194243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="4">
+        <v>107.38315919999999</v>
+      </c>
+      <c r="C50" s="4">
+        <v>10.7654198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="4">
+        <v>107.3296301</v>
+      </c>
+      <c r="C51" s="4">
+        <v>10.743019800000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="4">
+        <v>107.2914044</v>
+      </c>
+      <c r="C52" s="4">
+        <v>10.7994599</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="4"/>
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B73" s="4"/>
+      <c r="C73" s="4"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="4"/>
+      <c r="C82" s="4"/>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B83" s="4"/>
+      <c r="C83" s="4"/>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B84" s="4"/>
+      <c r="C84" s="4"/>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B88" s="4"/>
+      <c r="C88" s="4"/>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B89" s="4"/>
+      <c r="C89" s="4"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B94" s="4"/>
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B96" s="4"/>
+      <c r="C96" s="4"/>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B99" s="4"/>
+      <c r="C99" s="4"/>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B101" s="4"/>
+      <c r="C101" s="4"/>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Bo sung code dung OpenRouteService (ORS) free
</commit_message>
<xml_diff>
--- a/Scripts/data/input_location_data.xlsx
+++ b/Scripts/data/input_location_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SANG\Nam Project\python\CalcDistanceMatrixFromXY\Scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D326E8-4390-4406-B31C-DC7A99FC51F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6E9D504-2769-4AAB-AC55-5D6ACF95951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,10 +469,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>107.2925092</v>
+        <v>107.32507320000001</v>
       </c>
       <c r="C3" s="4">
-        <v>10.8382992</v>
+        <v>10.7692567</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -480,10 +480,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
-        <v>107.35621980000001</v>
+        <v>107.36582300000001</v>
       </c>
       <c r="C4" s="4">
-        <v>10.792846600000001</v>
+        <v>10.8321343</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -491,10 +491,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="4">
-        <v>107.3237412</v>
+        <v>107.35006660000001</v>
       </c>
       <c r="C5" s="4">
-        <v>10.723538400000001</v>
+        <v>10.827203000000001</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -502,10 +502,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="4">
-        <v>107.34938649999999</v>
+        <v>107.2939555</v>
       </c>
       <c r="C6" s="4">
-        <v>10.741887</v>
+        <v>10.827610999999999</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,10 +513,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="4">
-        <v>107.35160310000001</v>
+        <v>107.10463</v>
       </c>
       <c r="C7" s="4">
-        <v>10.7319087</v>
+        <v>10.7884175</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -524,10 +524,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="4">
-        <v>107.35157599999999</v>
+        <v>107.3888043</v>
       </c>
       <c r="C8" s="4">
-        <v>10.751467399999999</v>
+        <v>10.685542399999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -535,10 +535,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="4">
-        <v>107.35130100000001</v>
+        <v>107.2210231</v>
       </c>
       <c r="C9" s="4">
-        <v>10.747577700000001</v>
+        <v>10.7281704</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -546,10 +546,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="4">
-        <v>107.3512925</v>
+        <v>107.1958491</v>
       </c>
       <c r="C10" s="4">
-        <v>10.731367199999999</v>
+        <v>10.6897536</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -557,10 +557,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="4">
-        <v>107.3435336</v>
+        <v>107.1746567</v>
       </c>
       <c r="C11" s="4">
-        <v>10.7628431</v>
+        <v>10.680433000000001</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -568,10 +568,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="4">
-        <v>107.3505794</v>
+        <v>107.1782244</v>
       </c>
       <c r="C12" s="4">
-        <v>10.767490499999999</v>
+        <v>10.6571601</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,10 +579,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="4">
-        <v>107.3052122</v>
+        <v>107.1839014</v>
       </c>
       <c r="C13" s="4">
-        <v>10.7559752</v>
+        <v>10.729506900000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -590,10 +590,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="4">
-        <v>107.37694449999999</v>
+        <v>107.20045210000001</v>
       </c>
       <c r="C14" s="4">
-        <v>10.616922600000001</v>
+        <v>10.5933867</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -601,10 +601,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="4">
-        <v>107.54477369999999</v>
+        <v>107.1792863</v>
       </c>
       <c r="C15" s="4">
-        <v>10.559908500000001</v>
+        <v>10.5851787</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -612,10 +612,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="4">
-        <v>107.4345624</v>
+        <v>107.16441020000001</v>
       </c>
       <c r="C16" s="4">
-        <v>10.548318399999999</v>
+        <v>10.554601099999999</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -623,10 +623,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="4">
-        <v>107.3820486</v>
+        <v>107.4020519</v>
       </c>
       <c r="C17" s="4">
-        <v>10.8409555</v>
+        <v>10.9177465</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -634,10 +634,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="4">
-        <v>107.2201762</v>
+        <v>107.2610413</v>
       </c>
       <c r="C18" s="4">
-        <v>10.791483700000001</v>
+        <v>10.9208467</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -645,10 +645,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="4">
-        <v>107.1871233</v>
+        <v>107.2338276</v>
       </c>
       <c r="C19" s="4">
-        <v>10.8131679</v>
+        <v>10.9080052</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -656,10 +656,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="4">
-        <v>107.28000299999999</v>
+        <v>107.24312449999999</v>
       </c>
       <c r="C20" s="4">
-        <v>10.872092</v>
+        <v>10.921396</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -667,10 +667,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="4">
-        <v>107.1602683</v>
+        <v>107.2392042</v>
       </c>
       <c r="C21" s="4">
-        <v>10.8612799</v>
+        <v>10.937315</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -678,10 +678,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="4">
-        <v>107.2366997</v>
+        <v>107.2580737</v>
       </c>
       <c r="C22" s="4">
-        <v>10.8358981</v>
+        <v>10.946297700000001</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -689,10 +689,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="4">
-        <v>107.2304671</v>
+        <v>107.241535</v>
       </c>
       <c r="C23" s="4">
-        <v>10.8196677</v>
+        <v>10.956145599999999</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -700,10 +700,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="4">
-        <v>107.229674</v>
+        <v>107.2716479</v>
       </c>
       <c r="C24" s="4">
-        <v>10.817656700000001</v>
+        <v>10.942582399999999</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -711,10 +711,10 @@
         <v>23</v>
       </c>
       <c r="B25" s="4">
-        <v>107.23253219999999</v>
+        <v>107.2421288</v>
       </c>
       <c r="C25" s="4">
-        <v>10.824465399999999</v>
+        <v>10.940977500000001</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -722,10 +722,10 @@
         <v>24</v>
       </c>
       <c r="B26" s="4">
-        <v>107.2794317</v>
+        <v>107.2426289</v>
       </c>
       <c r="C26" s="4">
-        <v>10.696851799999999</v>
+        <v>10.9292567</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -733,10 +733,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="4">
-        <v>107.2416711</v>
+        <v>107.2584918</v>
       </c>
       <c r="C27" s="4">
-        <v>10.722218099999999</v>
+        <v>10.918987599999999</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -744,10 +744,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="4">
-        <v>107.2353122</v>
+        <v>107.2479385</v>
       </c>
       <c r="C28" s="4">
-        <v>10.7555388</v>
+        <v>10.923223999999999</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -755,10 +755,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="4">
-        <v>107.2386992</v>
+        <v>107.2392332</v>
       </c>
       <c r="C29" s="4">
-        <v>10.702419300000001</v>
+        <v>10.922207999999999</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -766,10 +766,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="4">
-        <v>107.24190919999999</v>
+        <v>107.2472046</v>
       </c>
       <c r="C30" s="4">
-        <v>10.631271699999999</v>
+        <v>10.928483399999999</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -777,10 +777,10 @@
         <v>29</v>
       </c>
       <c r="B31" s="4">
-        <v>107.07962790000001</v>
+        <v>107.25610159999999</v>
       </c>
       <c r="C31" s="4">
-        <v>10.6311929</v>
+        <v>10.9404308</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -788,10 +788,10 @@
         <v>30</v>
       </c>
       <c r="B32" s="4">
-        <v>107.06150909999999</v>
+        <v>107.2440003</v>
       </c>
       <c r="C32" s="4">
-        <v>10.6270311</v>
+        <v>10.940779300000001</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -799,10 +799,10 @@
         <v>31</v>
       </c>
       <c r="B33" s="4">
-        <v>107.2035956</v>
+        <v>107.2428219</v>
       </c>
       <c r="C33" s="4">
-        <v>10.7406097</v>
+        <v>10.9454365</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -810,10 +810,10 @@
         <v>32</v>
       </c>
       <c r="B34" s="4">
-        <v>107.1602683</v>
+        <v>107.2459412</v>
       </c>
       <c r="C34" s="4">
-        <v>10.730828199999999</v>
+        <v>10.6485699</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -821,10 +821,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="4">
-        <v>107.15105800000001</v>
+        <v>107.2408946</v>
       </c>
       <c r="C35" s="4">
-        <v>10.723762499999999</v>
+        <v>10.6486074</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -832,10 +832,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="4">
-        <v>107.1535451</v>
+        <v>107.23867439999999</v>
       </c>
       <c r="C36" s="4">
-        <v>10.719318400000001</v>
+        <v>10.6492456</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -843,10 +843,10 @@
         <v>35</v>
       </c>
       <c r="B37" s="4">
-        <v>107.13278560000001</v>
+        <v>107.24345049999999</v>
       </c>
       <c r="C37" s="4">
-        <v>10.8292514</v>
+        <v>10.6388149</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -854,10 +854,10 @@
         <v>36</v>
       </c>
       <c r="B38" s="4">
-        <v>107.0845808</v>
+        <v>107.455218</v>
       </c>
       <c r="C38" s="4">
-        <v>10.817228800000001</v>
+        <v>10.866531800000001</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,10 +865,10 @@
         <v>37</v>
       </c>
       <c r="B39" s="4">
-        <v>107.03782630000001</v>
+        <v>107.3956658</v>
       </c>
       <c r="C39" s="4">
-        <v>10.998201699999999</v>
+        <v>10.912235600000001</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -876,10 +876,10 @@
         <v>38</v>
       </c>
       <c r="B40" s="4">
-        <v>107.31226359999999</v>
+        <v>107.2765575</v>
       </c>
       <c r="C40" s="4">
-        <v>10.807557900000001</v>
+        <v>10.9008602</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -887,10 +887,10 @@
         <v>39</v>
       </c>
       <c r="B41" s="4">
-        <v>107.29619529999999</v>
+        <v>107.185294</v>
       </c>
       <c r="C41" s="4">
-        <v>10.815440600000001</v>
+        <v>10.9406493</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -898,10 +898,10 @@
         <v>40</v>
       </c>
       <c r="B42" s="4">
-        <v>107.29703499999999</v>
+        <v>107.19187429999999</v>
       </c>
       <c r="C42" s="4">
-        <v>10.834960000000001</v>
+        <v>10.871928799999999</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -909,10 +909,10 @@
         <v>41</v>
       </c>
       <c r="B43" s="4">
-        <v>107.2838081</v>
+        <v>107.17799359999999</v>
       </c>
       <c r="C43" s="4">
-        <v>10.902956400000001</v>
+        <v>10.9092302</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -920,10 +920,10 @@
         <v>42</v>
       </c>
       <c r="B44" s="4">
-        <v>107.3682</v>
+        <v>107.1839643</v>
       </c>
       <c r="C44" s="4">
-        <v>10.762578</v>
+        <v>10.9301808</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -931,10 +931,10 @@
         <v>43</v>
       </c>
       <c r="B45" s="4">
-        <v>107.332729</v>
+        <v>107.1874938</v>
       </c>
       <c r="C45" s="4">
-        <v>10.7147962</v>
+        <v>10.9248201</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -942,10 +942,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="4">
-        <v>107.3257545</v>
+        <v>107.185277</v>
       </c>
       <c r="C46" s="4">
-        <v>10.6997304</v>
+        <v>10.925613</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -953,10 +953,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="4">
-        <v>107.312364</v>
+        <v>107.2295735</v>
       </c>
       <c r="C47" s="4">
-        <v>10.67906</v>
+        <v>10.901373599999999</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -964,10 +964,10 @@
         <v>46</v>
       </c>
       <c r="B48" s="4">
-        <v>107.34070149999999</v>
+        <v>107.1996238</v>
       </c>
       <c r="C48" s="4">
-        <v>10.7179792</v>
+        <v>10.8768876</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -975,10 +975,10 @@
         <v>47</v>
       </c>
       <c r="B49" s="4">
-        <v>107.33578300000001</v>
+        <v>107.2499741</v>
       </c>
       <c r="C49" s="4">
-        <v>10.7194243</v>
+        <v>10.919068599999999</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -986,10 +986,10 @@
         <v>48</v>
       </c>
       <c r="B50" s="4">
-        <v>107.38315919999999</v>
+        <v>107.2321755</v>
       </c>
       <c r="C50" s="4">
-        <v>10.7654198</v>
+        <v>10.9057944</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -997,10 +997,10 @@
         <v>49</v>
       </c>
       <c r="B51" s="4">
-        <v>107.3296301</v>
+        <v>107.23705699999999</v>
       </c>
       <c r="C51" s="4">
-        <v>10.743019800000001</v>
+        <v>10.958171999999999</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1008,10 +1008,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="4">
-        <v>107.2914044</v>
+        <v>107.2186164</v>
       </c>
       <c r="C52" s="4">
-        <v>10.7994599</v>
+        <v>10.9654609</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>